<commit_message>
generation et ajout tracking number. eliminer la commande deja créée dans mode manuel.
</commit_message>
<xml_diff>
--- a/src/assets/DATA/05-12-2021/Facture/commande1.xlsx
+++ b/src/assets/DATA/05-12-2021/Facture/commande1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DATA\05-12-2021\Facture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898A163B-6969-4AB2-B04D-EB75E58757C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C43230-E8D9-4FB6-9D7F-15EF43194941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>reference</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>produit 4G</t>
+  </si>
+  <si>
+    <t>etat commande TMS</t>
+  </si>
+  <si>
+    <t>valide</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="Q1" sqref="Q1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,9 +471,10 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,8 +523,11 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -566,8 +576,11 @@
       <c r="P2">
         <v>30</v>
       </c>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -596,7 +609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>

</xml_diff>